<commit_message>
Read channel names dynamically from Summary sheet
Instead of hardcoding channel names (Retail, Subscription, Pool), parse
them from the "Payments by Channel" section in the Summary sheet. This
handles reports with different or additional channels.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/partners/tests/data/Bad Report.xlsx
+++ b/partners/tests/data/Bad Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Retail" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Unexpected" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Subscription" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Pool" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="92">
   <si>
     <t xml:space="preserve">Payee Name:</t>
   </si>
@@ -73,76 +73,79 @@
     <t xml:space="preserve">Royalty Payment</t>
   </si>
   <si>
+    <t xml:space="preserve">Unexpected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subscription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royalty Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISBN #</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promotion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sale Territory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DLP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royalty Earned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less Distribution Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royalty Payable Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Royalty Payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Палёт над гняздом зязюлі</t>
+  </si>
+  <si>
     <t xml:space="preserve">Retail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subscription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Royalty Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISBN #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publisher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promotion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sale Territory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DLP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sales Qty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Royalty Earned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Less Distribution Fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exchange Rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Royalty Payable Currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Royalty Payable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Палёт над гняздом зязюлі</t>
   </si>
   <si>
     <t xml:space="preserve">CD5216806</t>
@@ -504,8 +507,8 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -628,10 +631,10 @@
   </sheetPr>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
+      <selection pane="bottomLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,25 +709,25 @@
         <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>17</v>
@@ -733,7 +736,7 @@
         <v>12</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>1</v>
@@ -757,28 +760,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>17</v>
@@ -787,7 +790,7 @@
         <v>10</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M3" s="5" t="n">
         <v>1</v>
@@ -811,28 +814,28 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>17</v>
@@ -841,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>1</v>
@@ -865,28 +868,28 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>17</v>
@@ -895,7 +898,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>1</v>
@@ -1160,28 +1163,28 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>0.4</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>17</v>
@@ -1190,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>1</v>
@@ -1214,28 +1217,28 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4" t="n">
         <v>0.4</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>17</v>
@@ -1244,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M3" s="5" t="n">
         <v>1</v>
@@ -1268,28 +1271,28 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="4" t="n">
         <v>0.4</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>17</v>
@@ -1298,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" s="5" t="n">
         <v>1</v>
@@ -1322,28 +1325,28 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4" t="n">
         <v>0.4</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>17</v>
@@ -1352,7 +1355,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M5" s="5" t="n">
         <v>1</v>
@@ -1376,28 +1379,28 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>0.4</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>17</v>
@@ -1406,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M6" s="5" t="n">
         <v>1</v>
@@ -1522,26 +1525,26 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>17</v>
@@ -1550,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" s="5" t="n">
         <v>0</v>
@@ -1572,26 +1575,26 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>17</v>
@@ -1600,7 +1603,7 @@
         <v>15</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M3" s="5" t="n">
         <v>0</v>

</xml_diff>